<commit_message>
feat: add proxy support for Playwright and curl-cffi, update selectors for Avito, update .env example
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,56 @@
         <v>435</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/all/predlozheniya_uslug?cd=1&amp;q=программист+python</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>программист python во всех регионах - цены и отзывы | Услуги на Авито | Поиск специалистов</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>программист python во всех регионах - цены и отзывы | Услуги на Авито | Поиск специалистов Как дальше пользоваться Авито на iOS. Подробнее Для бизнеса Продавать Покупать Нанимать Карьера в Авито Помощь Каталоги Каталог автомобилей Каталог новостроек #яПомогаю Избранное Корзина Вход и регистрация Разместить объявление Все категории программист python Найти Во всех регионах Главная Услуги Предложение услуг программист python «программист python»: объявления 1 448 Показать объявления на карте Сортировка Сохранить поиск Программист 1С: настройка, обновление, консультаци Цена договорная Разработка CRM-систем от 1 000 ₽ Разработка на Python от 1 000 ₽ Ещё 5 услуг Смоленская обл., Сафоновский муниципальный округ, Сафоново Обо мне:
+Опыт работы с 1С: более 10 лет.
+Работаю напрямую с клиентом (без посредников).
+Все официальные сертификаты 1С есть в наличии (см. Фото).
+Нацелен на долгосрочное и качественное сотрудничество.
+Перечень основных конфигураций, с которыми я ра... Продвинуто Программис</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/all/predlozheniya_uslug?cd=1&amp;q=программист+python</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>программист python во всех регионах - цены и отзывы | Услуги на Авито | Поиск специалистов</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>программист python во всех регионах - цены и отзывы | Услуги на Авито | Поиск специалистов Как дальше пользоваться Авито на iOS. Подробнее Для бизнеса Продавать Покупать Нанимать Карьера в Авито Помощь Каталоги Каталог автомобилей Каталог новостроек #яПомогаю Избранное Корзина Вход и регистрация Разместить объявление Все категории программист python Найти Во всех регионах Главная Услуги Предложение услуг программист python «программист python»: объявления 1 451 Показать объявления на карте Сортировка Сохранить поиск Программист 1С: настройка, обновление, консультаци Цена договорная Разработка CRM-систем от 1 000 ₽ Разработка на Python от 1 000 ₽ Ещё 5 услуг Смоленская обл., Сафоновский муниципальный округ, Сафоново Обо мне:
+Опыт работы с 1С: более 10 лет.
+Работаю напрямую с клиентом (без посредников).
+Все официальные сертификаты 1С есть в наличии (см. Фото).
+Нацелен на долгосрочное и качественное сотрудничество.
+Перечень основных конфигураций, с которыми я ра... Продвинуто Программис</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>436</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>